<commit_message>
conectando modulo de contadores al front
</commit_message>
<xml_diff>
--- a/backend/app/modules/registro_contadores/registros.xlsx
+++ b/backend/app/modules/registro_contadores/registros.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col width="19.28515625" customWidth="1" min="1" max="1"/>
+    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="15.28515625" customWidth="1" min="3" max="3"/>
+    <col width="15.85546875" customWidth="1" min="4" max="4"/>
+    <col width="15.28515625" customWidth="1" min="5" max="5"/>
+    <col width="13.85546875" customWidth="1" min="6" max="6"/>
+    <col width="17" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -456,6 +464,64 @@
         <is>
           <t>Billetero</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Casino Medellín</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>M1-1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>200000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Casino Medellín</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>M1-1</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>